<commit_message>
improving plot annotation and added a packages requirements file
</commit_message>
<xml_diff>
--- a/SCALARSelectedandConvertedStatements_PA.xlsx
+++ b/SCALARSelectedandConvertedStatements_PA.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="72">
   <si>
     <t>Attribute</t>
   </si>
@@ -50,31 +50,58 @@
     <t>People living in the Netherlands</t>
   </si>
   <si>
+    <t>R2_implementation_SM1</t>
+  </si>
+  <si>
+    <t>R2_implementation_SM2</t>
+  </si>
+  <si>
     <t>R2_implementation_SM3</t>
   </si>
   <si>
-    <t>R2_implementation_SM6</t>
-  </si>
-  <si>
-    <t>(None,)</t>
+    <t>R2_implementation_NM2</t>
+  </si>
+  <si>
+    <t>R2_implementation_NM3</t>
+  </si>
+  <si>
+    <t>R2_implementation_NM6</t>
+  </si>
+  <si>
+    <t>R1c_perc_cost_SM1</t>
+  </si>
+  <si>
+    <t>R05_worry</t>
+  </si>
+  <si>
+    <t>Q0_age</t>
+  </si>
+  <si>
+    <t>R1c_perc_cost_SM2</t>
+  </si>
+  <si>
+    <t>R1a_self_efficacy_SM3</t>
   </si>
   <si>
     <t>R1c_perc_cost_SM3</t>
   </si>
   <si>
-    <t>R1a_self_efficacy_SM3</t>
-  </si>
-  <si>
-    <t>R1c_perc_cost_SM6</t>
-  </si>
-  <si>
-    <t>R1a_self_efficacy_SM6</t>
-  </si>
-  <si>
-    <t>R01_resilience_6</t>
-  </si>
-  <si>
-    <t>R08_economic_comfort</t>
+    <t>R1c_perc_cost_NM3</t>
+  </si>
+  <si>
+    <t>R1a_self_efficacy_NM6</t>
+  </si>
+  <si>
+    <t>R1a_self_efficacy_SM1</t>
+  </si>
+  <si>
+    <t>R1a_self_efficacy_SM2</t>
+  </si>
+  <si>
+    <t>R1a_self_efficacy_NM3</t>
+  </si>
+  <si>
+    <t>R1c_perc_cost_NM6</t>
   </si>
   <si>
     <t>Aim_description</t>
@@ -98,64 +125,112 @@
     <t>final_entropy</t>
   </si>
   <si>
+    <t>Raising the level of the ground floor above the most likely flood level, Please indicate if you have already implemented any of these structural measures or if you intend to do so in the future</t>
+  </si>
+  <si>
+    <t>Strengthen the housing foundations to withstand water pressures, Please indicate if you have already implemented any of these structural measures or if you intend to do so in the future</t>
+  </si>
+  <si>
     <t>Reconstructing or reinforcing the walls and/or the ground floor with water-resistant materials, Please indicate if you have already implemented any of these structural measures or if you intend to do so in the future</t>
   </si>
   <si>
-    <t>Installing a pump and/or one or more system(s) to drain flood water, Please indicate if you have already implemented any of these structural measures or if you intend to do so in the future</t>
+    <t>Purchasing sandbags, or other water barriers, Please indicate if you have already implemented any of these nonstructural measures or if you intend to do so in the future</t>
+  </si>
+  <si>
+    <t>Buying a spare power generator to power your home, Please indicate if you have already implemented any of these nonstructural measures or if you intend to do so in the future</t>
+  </si>
+  <si>
+    <t>Installing a refuge zone, or an opening in the roof of your home or apartment, Please indicate if you have already implemented any of these nonstructural measures or if you intend to do so in the future</t>
+  </si>
+  <si>
+    <t>not raise the level of the ground floor above the most likely flood level within the next year</t>
+  </si>
+  <si>
+    <t>not strengthen the housing foundations to withstand water pressures</t>
   </si>
   <si>
     <t>not reconstruct or reinforce walls and/or ground floor with water-resistant materials within the next year</t>
   </si>
   <si>
-    <t>not install a pump and/or one or more systems to drain flood water within the next year</t>
+    <t>not purchase sandbags or other water barriers within the next year</t>
+  </si>
+  <si>
+    <t>not buy a spare power generator to power their home within the next year</t>
+  </si>
+  <si>
+    <t>not install a refuge zone in their home or apartment within the next year</t>
+  </si>
+  <si>
+    <t>Raising the level of the ground floor above the most likely flood level, When you think in terms of your income and your other expenses, do you believe that implementing or paying someone to implement this structural measure would be cheap or expensive?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How worried or not are you about the potential impact of flooding on your home?, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age, </t>
+  </si>
+  <si>
+    <t>Strengthen the housing foundations to withstand water pressures, When you think in terms of your income and your other expenses, do you believe that implementing or paying someone to implement this structural measure would be cheap or expensive?</t>
+  </si>
+  <si>
+    <t>Reconstructing or reinforcing the walls and/or the ground floor with water-resistant materials, Do you have the ability to undertake the structural measure either yourself or by paying a professional to do so?</t>
   </si>
   <si>
     <t>Reconstructing or reinforcing the walls and/or the ground floor with water-resistant materials, When you think in terms of your income and your other expenses, do you believe that implementing or paying someone to implement this structural measure would be cheap or expensive?</t>
   </si>
   <si>
-    <t>Reconstructing or reinforcing the walls and/or the ground floor with water-resistant materials, Do you have the ability to undertake the structural measure either yourself or by paying a professional to do so?</t>
-  </si>
-  <si>
-    <t>Installing a pump and/or one or more system(s) to drain flood water, When you think in terms of your income and your other expenses, do you believe that implementing or paying someone to implement this structural measure would be cheap or expensive?</t>
-  </si>
-  <si>
-    <t>Installing a pump and/or one or more system(s) to drain flood water, Do you have the ability to undertake the structural measure either yourself or by paying a professional to do so?</t>
+    <t>Buying a spare power generator to power your home, When you think in terms of your income and your other expenses, do you believe that implementing or paying someone to implement this nonstructural measure would be cheap or expensive?</t>
+  </si>
+  <si>
+    <t>Installing a refuge zone, or an opening in the roof of your home or apartment, Do you have the ability to undertake the nonstructural measure either yourself or by paying a professional to do so?</t>
+  </si>
+  <si>
+    <t>if they believe that implementing or paying someone to implement this structural measure would be expensive</t>
+  </si>
+  <si>
+    <t>if they are not worried about the potential impact of flooding on their home</t>
+  </si>
+  <si>
+    <t>if they are younger than 45</t>
+  </si>
+  <si>
+    <t>if they are older than 45</t>
+  </si>
+  <si>
+    <t>if they are not able to undertake the structural measure either themselves or by paying a professional to do so</t>
+  </si>
+  <si>
+    <t>if they believe that implementing or paying someone to implement this nonstructural measure would be expensive</t>
+  </si>
+  <si>
+    <t>if they are not able to install a refuge zone or an opening in the roof of their home or apartment</t>
+  </si>
+  <si>
+    <t>Raising the level of the ground floor above the most likely flood level</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Strengthen the housing foundations to withstand water pressures</t>
+  </si>
+  <si>
+    <t>Reconstructing or reinforcing the walls and/or the ground floor with water-resistant materials</t>
+  </si>
+  <si>
+    <t>Buying a spare power generator to power your home</t>
+  </si>
+  <si>
+    <t>Installing a refuge zone, or an opening in the roof of your home or apartment</t>
   </si>
   <si>
     <t>None</t>
   </si>
   <si>
-    <t>if they believe that implementing or paying someone to implement this structural measure would be cheap</t>
-  </si>
-  <si>
-    <t>if they believe that implementing or paying someone to implement this structural measure would be expensive</t>
-  </si>
-  <si>
-    <t>if they are not able to undertake the structural measure either themselves or by paying a professional to do so</t>
-  </si>
-  <si>
-    <t>if they do not have the ability to undertake the structural measure either themselves or by paying a professional to do so</t>
-  </si>
-  <si>
-    <t>My household can rely on the support from my government when I need help (e.g. receiving funding or support in the event of a natural disaster)</t>
-  </si>
-  <si>
-    <t>Reconstructing or reinforcing the walls and/or the ground floor with water-resistant materials</t>
-  </si>
-  <si>
-    <t>When considering your salary along with your expenses, how would you describe your level of 'economic comfort'?</t>
-  </si>
-  <si>
-    <t>Installing a pump and/or one or more system(s) to drain flood water</t>
-  </si>
-  <si>
-    <t>if they feel they can rely on government support</t>
-  </si>
-  <si>
-    <t>if they feel they cannot rely on government support</t>
-  </si>
-  <si>
-    <t>if they feel they are not living comfortably</t>
+    <t>if they are not able to</t>
+  </si>
+  <si>
+    <t>if they are not able to buy a spare power generator to power their home</t>
   </si>
 </sst>
 </file>
@@ -513,7 +588,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -559,28 +634,25 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D2">
-        <v>0.8930112165660051</v>
+        <v>0.7684426229508197</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F2">
-        <v>1159</v>
+        <v>632</v>
       </c>
       <c r="G2">
-        <v>0.8930112165660051</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
+        <v>0.8908227848101266</v>
       </c>
       <c r="I2">
-        <v>1159</v>
+        <v>632</v>
       </c>
       <c r="J2">
-        <v>0.8930112165660051</v>
+        <v>0.8908227848101266</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -591,28 +663,28 @@
         <v>11</v>
       </c>
       <c r="C3">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D3">
-        <v>0.8930112165660051</v>
+        <v>0.7684426229508197</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F3">
-        <v>416</v>
+        <v>632</v>
       </c>
       <c r="G3">
-        <v>0.7788461538461539</v>
+        <v>0.8908227848101266</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I3">
-        <v>311</v>
+        <v>572</v>
       </c>
       <c r="J3">
-        <v>0.7877813504823151</v>
+        <v>0.9265734265734266</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -623,25 +695,25 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D4">
-        <v>0.8930112165660051</v>
+        <v>0.7684426229508197</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F4">
-        <v>743</v>
+        <v>863</v>
       </c>
       <c r="G4">
-        <v>0.9569313593539704</v>
+        <v>0.813441483198146</v>
       </c>
       <c r="I4">
-        <v>743</v>
+        <v>863</v>
       </c>
       <c r="J4">
-        <v>0.9569313593539704</v>
+        <v>0.813441483198146</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -652,28 +724,28 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D5">
-        <v>0.8930112165660051</v>
+        <v>0.7684426229508197</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F5">
-        <v>743</v>
+        <v>863</v>
       </c>
       <c r="G5">
-        <v>0.9569313593539704</v>
+        <v>0.813441483198146</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I5">
-        <v>635</v>
+        <v>381</v>
       </c>
       <c r="J5">
-        <v>0.9732283464566929</v>
+        <v>0.916010498687664</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -681,28 +753,31 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D6">
-        <v>0.8930112165660051</v>
+        <v>0.7725409836065574</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F6">
-        <v>974</v>
+        <v>564</v>
       </c>
       <c r="G6">
-        <v>0.9065708418891171</v>
+        <v>0.6790780141843972</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
       </c>
       <c r="I6">
-        <v>974</v>
+        <v>357</v>
       </c>
       <c r="J6">
-        <v>0.9065708418891171</v>
+        <v>0.7871148459383753</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -710,31 +785,28 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D7">
-        <v>0.8930112165660051</v>
+        <v>0.7725409836065574</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F7">
-        <v>974</v>
+        <v>412</v>
       </c>
       <c r="G7">
-        <v>0.9065708418891171</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
+        <v>0.9004854368932039</v>
       </c>
       <c r="I7">
-        <v>680</v>
+        <v>412</v>
       </c>
       <c r="J7">
-        <v>0.9058823529411765</v>
+        <v>0.9004854368932039</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -742,31 +814,31 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D8">
-        <v>0.8930112165660051</v>
+        <v>0.7725409836065574</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F8">
-        <v>974</v>
+        <v>412</v>
       </c>
       <c r="G8">
-        <v>0.9065708418891171</v>
+        <v>0.9004854368932039</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I8">
-        <v>294</v>
+        <v>387</v>
       </c>
       <c r="J8">
-        <v>0.9081632653061225</v>
+        <v>0.9198966408268734</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -777,28 +849,25 @@
         <v>12</v>
       </c>
       <c r="C9">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D9">
-        <v>0.8731665228645384</v>
+        <v>0.7725409836065574</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F9">
-        <v>1159</v>
+        <v>654</v>
       </c>
       <c r="G9">
-        <v>0.8731665228645384</v>
-      </c>
-      <c r="H9" t="s">
-        <v>13</v>
+        <v>0.8532110091743119</v>
       </c>
       <c r="I9">
-        <v>1159</v>
+        <v>654</v>
       </c>
       <c r="J9">
-        <v>0.8731665228645384</v>
+        <v>0.8532110091743119</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -809,25 +878,28 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D10">
-        <v>0.8731665228645384</v>
+        <v>0.7725409836065574</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F10">
-        <v>572</v>
+        <v>654</v>
       </c>
       <c r="G10">
-        <v>0.8234265734265734</v>
+        <v>0.8532110091743119</v>
+      </c>
+      <c r="H10" t="s">
+        <v>26</v>
       </c>
       <c r="I10">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J10">
-        <v>0.8234265734265734</v>
+        <v>0.8896672504378283</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -835,31 +907,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D11">
-        <v>0.8731665228645384</v>
+        <v>0.757172131147541</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F11">
-        <v>572</v>
+        <v>822</v>
       </c>
       <c r="G11">
-        <v>0.8234265734265734</v>
-      </c>
-      <c r="H11" t="s">
-        <v>19</v>
+        <v>0.818734793187348</v>
       </c>
       <c r="I11">
-        <v>291</v>
+        <v>822</v>
       </c>
       <c r="J11">
-        <v>0.8075601374570447</v>
+        <v>0.818734793187348</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -867,28 +936,31 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D12">
-        <v>0.8731665228645384</v>
+        <v>0.757172131147541</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F12">
-        <v>587</v>
+        <v>822</v>
       </c>
       <c r="G12">
-        <v>0.9216354344122658</v>
+        <v>0.818734793187348</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
       </c>
       <c r="I12">
-        <v>587</v>
+        <v>537</v>
       </c>
       <c r="J12">
-        <v>0.9216354344122658</v>
+        <v>0.9199255121042831</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -896,31 +968,28 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D13">
-        <v>0.8731665228645384</v>
+        <v>0.757172131147541</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F13">
-        <v>587</v>
+        <v>633</v>
       </c>
       <c r="G13">
-        <v>0.9216354344122658</v>
-      </c>
-      <c r="H13" t="s">
-        <v>17</v>
+        <v>0.8499210110584519</v>
       </c>
       <c r="I13">
-        <v>468</v>
+        <v>633</v>
       </c>
       <c r="J13">
-        <v>0.9487179487179487</v>
+        <v>0.8499210110584519</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -928,28 +997,31 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C14">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D14">
-        <v>0.8731665228645384</v>
+        <v>0.6987704918032787</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F14">
-        <v>911</v>
+        <v>863</v>
       </c>
       <c r="G14">
-        <v>0.8902305159165752</v>
+        <v>0.7323290845886443</v>
+      </c>
+      <c r="H14" t="s">
+        <v>19</v>
       </c>
       <c r="I14">
-        <v>911</v>
+        <v>381</v>
       </c>
       <c r="J14">
-        <v>0.8902305159165752</v>
+        <v>0.8083989501312336</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -957,31 +1029,63 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C15">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D15">
-        <v>0.8731665228645384</v>
+        <v>0.6875</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F15">
-        <v>911</v>
+        <v>606</v>
       </c>
       <c r="G15">
-        <v>0.8902305159165752</v>
+        <v>0.7557755775577558</v>
       </c>
       <c r="H15" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="I15">
-        <v>644</v>
+        <v>425</v>
       </c>
       <c r="J15">
-        <v>0.8850931677018633</v>
+        <v>0.8188235294117647</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>976</v>
+      </c>
+      <c r="D16">
+        <v>0.6926229508196722</v>
+      </c>
+      <c r="E16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16">
+        <v>743</v>
+      </c>
+      <c r="G16">
+        <v>0.7402422611036339</v>
+      </c>
+      <c r="H16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16">
+        <v>413</v>
+      </c>
+      <c r="J16">
+        <v>0.8087167070217918</v>
       </c>
     </row>
   </sheetData>
@@ -991,7 +1095,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1005,10 +1109,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1020,10 +1124,10 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>5</v>
@@ -1035,10 +1139,10 @@
         <v>7</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>8</v>
@@ -1047,7 +1151,7 @@
         <v>9</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1058,43 +1162,43 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="E2">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F2">
-        <v>0.8930112165660051</v>
+        <v>0.7684426229508197</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>48</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="J2">
-        <v>1159</v>
+        <v>632</v>
       </c>
       <c r="K2">
-        <v>0.8930112165660051</v>
-      </c>
-      <c r="L2" t="s">
-        <v>13</v>
+        <v>0.8908227848101266</v>
       </c>
       <c r="N2" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="O2">
-        <v>1159</v>
+        <v>632</v>
       </c>
       <c r="P2">
-        <v>0.8930112165660051</v>
+        <v>0.8908227848101266</v>
       </c>
       <c r="Q2">
-        <v>0.4907658676516883</v>
+        <v>0.4974291918181426</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1105,49 +1209,49 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="E3">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F3">
-        <v>0.8930112165660051</v>
+        <v>0.7684426229508197</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="J3">
-        <v>416</v>
+        <v>632</v>
       </c>
       <c r="K3">
-        <v>0.7788461538461539</v>
+        <v>0.8908227848101266</v>
       </c>
       <c r="L3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="M3" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="N3" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="O3">
-        <v>311</v>
+        <v>572</v>
       </c>
       <c r="P3">
-        <v>0.7877813504823151</v>
+        <v>0.9265734265734266</v>
       </c>
       <c r="Q3">
-        <v>0.7457022590910922</v>
+        <v>0.3785827651603728</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1158,43 +1262,43 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="E4">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F4">
-        <v>0.8930112165660051</v>
+        <v>0.7684426229508197</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="I4" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="J4">
-        <v>743</v>
+        <v>863</v>
       </c>
       <c r="K4">
-        <v>0.9569313593539704</v>
+        <v>0.813441483198146</v>
       </c>
       <c r="N4" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="O4">
-        <v>743</v>
+        <v>863</v>
       </c>
       <c r="P4">
-        <v>0.9569313593539704</v>
+        <v>0.813441483198146</v>
       </c>
       <c r="Q4">
-        <v>0.256189076205616</v>
+        <v>0.6942163713918693</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -1205,49 +1309,49 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="E5">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F5">
-        <v>0.8930112165660051</v>
+        <v>0.7684426229508197</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="J5">
-        <v>743</v>
+        <v>863</v>
       </c>
       <c r="K5">
-        <v>0.9569313593539704</v>
+        <v>0.813441483198146</v>
       </c>
       <c r="L5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="M5" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="N5" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="O5">
-        <v>635</v>
+        <v>381</v>
       </c>
       <c r="P5">
-        <v>0.9732283464566929</v>
+        <v>0.916010498687664</v>
       </c>
       <c r="Q5">
-        <v>0.1779340107206948</v>
+        <v>0.4160827624351366</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1255,46 +1359,52 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E6">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F6">
-        <v>0.8930112165660051</v>
+        <v>0.7725409836065574</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="J6">
-        <v>974</v>
+        <v>564</v>
       </c>
       <c r="K6">
-        <v>0.9065708418891171</v>
+        <v>0.6790780141843972</v>
+      </c>
+      <c r="L6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" t="s">
+        <v>65</v>
       </c>
       <c r="N6" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="O6">
-        <v>974</v>
+        <v>357</v>
       </c>
       <c r="P6">
-        <v>0.9065708418891171</v>
+        <v>0.7871148459383753</v>
       </c>
       <c r="Q6">
-        <v>0.4478134923988957</v>
+        <v>0.7469615329260388</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1302,52 +1412,46 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E7">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F7">
-        <v>0.8930112165660051</v>
+        <v>0.7725409836065574</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="J7">
-        <v>974</v>
+        <v>412</v>
       </c>
       <c r="K7">
-        <v>0.9065708418891171</v>
-      </c>
-      <c r="L7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7" t="s">
-        <v>40</v>
+        <v>0.9004854368932039</v>
       </c>
       <c r="N7" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="O7">
-        <v>680</v>
+        <v>412</v>
       </c>
       <c r="P7">
-        <v>0.9058823529411765</v>
+        <v>0.9004854368932039</v>
       </c>
       <c r="Q7">
-        <v>0.4500666580964382</v>
+        <v>0.4674549036015206</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1355,52 +1459,52 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E8">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F8">
-        <v>0.8930112165660051</v>
+        <v>0.7725409836065574</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="I8" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="J8">
-        <v>974</v>
+        <v>412</v>
       </c>
       <c r="K8">
-        <v>0.9065708418891171</v>
+        <v>0.9004854368932039</v>
       </c>
       <c r="L8" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="M8" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="N8" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="O8">
-        <v>294</v>
+        <v>387</v>
       </c>
       <c r="P8">
-        <v>0.9081632653061225</v>
+        <v>0.9198966408268734</v>
       </c>
       <c r="Q8">
-        <v>0.4425710648397979</v>
+        <v>0.4025432779892922</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1411,43 +1515,43 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E9">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F9">
-        <v>0.8731665228645384</v>
+        <v>0.7725409836065574</v>
       </c>
       <c r="G9" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>51</v>
       </c>
       <c r="I9" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="J9">
-        <v>1159</v>
+        <v>654</v>
       </c>
       <c r="K9">
-        <v>0.8731665228645384</v>
-      </c>
-      <c r="L9" t="s">
-        <v>13</v>
+        <v>0.8532110091743119</v>
       </c>
       <c r="N9" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="O9">
-        <v>1159</v>
+        <v>654</v>
       </c>
       <c r="P9">
-        <v>0.8731665228645384</v>
+        <v>0.8532110091743119</v>
       </c>
       <c r="Q9">
-        <v>0.5486895858799942</v>
+        <v>0.6017460730975969</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1458,43 +1562,49 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E10">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F10">
-        <v>0.8731665228645384</v>
+        <v>0.7725409836065574</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H10" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="I10" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="J10">
-        <v>572</v>
+        <v>654</v>
       </c>
       <c r="K10">
-        <v>0.8234265734265734</v>
+        <v>0.8532110091743119</v>
+      </c>
+      <c r="L10" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" t="s">
+        <v>65</v>
       </c>
       <c r="N10" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="O10">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="P10">
-        <v>0.8234265734265734</v>
+        <v>0.8896672504378283</v>
       </c>
       <c r="Q10">
-        <v>0.6725233117337178</v>
+        <v>0.5009188161671247</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1502,52 +1612,46 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E11">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F11">
-        <v>0.8731665228645384</v>
+        <v>0.757172131147541</v>
       </c>
       <c r="G11" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H11" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="I11" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="J11">
-        <v>572</v>
+        <v>822</v>
       </c>
       <c r="K11">
-        <v>0.8234265734265734</v>
-      </c>
-      <c r="L11" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" t="s">
-        <v>42</v>
+        <v>0.818734793187348</v>
       </c>
       <c r="N11" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="O11">
-        <v>291</v>
+        <v>822</v>
       </c>
       <c r="P11">
-        <v>0.8075601374570447</v>
+        <v>0.818734793187348</v>
       </c>
       <c r="Q11">
-        <v>0.7065476519185905</v>
+        <v>0.6828370374266884</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1555,46 +1659,52 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E12">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F12">
-        <v>0.8731665228645384</v>
+        <v>0.757172131147541</v>
       </c>
       <c r="G12" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H12" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="I12" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="J12">
-        <v>587</v>
+        <v>822</v>
       </c>
       <c r="K12">
-        <v>0.9216354344122658</v>
+        <v>0.818734793187348</v>
+      </c>
+      <c r="L12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" t="s">
+        <v>66</v>
       </c>
       <c r="N12" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="O12">
-        <v>587</v>
+        <v>537</v>
       </c>
       <c r="P12">
-        <v>0.9216354344122658</v>
+        <v>0.9199255121042831</v>
       </c>
       <c r="Q12">
-        <v>0.3963902569449249</v>
+        <v>0.4024415985533437</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1602,52 +1712,46 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E13">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F13">
-        <v>0.8731665228645384</v>
+        <v>0.757172131147541</v>
       </c>
       <c r="G13" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H13" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="I13" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="J13">
-        <v>587</v>
+        <v>633</v>
       </c>
       <c r="K13">
-        <v>0.9216354344122658</v>
-      </c>
-      <c r="L13" t="s">
-        <v>17</v>
-      </c>
-      <c r="M13" t="s">
-        <v>43</v>
+        <v>0.8499210110584519</v>
       </c>
       <c r="N13" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="O13">
-        <v>468</v>
+        <v>633</v>
       </c>
       <c r="P13">
-        <v>0.9487179487179487</v>
+        <v>0.8499210110584519</v>
       </c>
       <c r="Q13">
-        <v>0.2918182565988858</v>
+        <v>0.6100379392752546</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1655,46 +1759,52 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E14">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F14">
-        <v>0.8731665228645384</v>
+        <v>0.6987704918032787</v>
       </c>
       <c r="G14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H14" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="I14" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="J14">
-        <v>911</v>
+        <v>863</v>
       </c>
       <c r="K14">
-        <v>0.8902305159165752</v>
+        <v>0.7323290845886443</v>
+      </c>
+      <c r="L14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" t="s">
+        <v>64</v>
       </c>
       <c r="N14" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="O14">
-        <v>911</v>
+        <v>381</v>
       </c>
       <c r="P14">
-        <v>0.8902305159165752</v>
+        <v>0.8083989501312336</v>
       </c>
       <c r="Q14">
-        <v>0.4992202608188665</v>
+        <v>0.7048087430516662</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1702,52 +1812,105 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15">
+        <v>976</v>
+      </c>
+      <c r="F15">
+        <v>0.6875</v>
+      </c>
+      <c r="G15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15">
+        <v>606</v>
+      </c>
+      <c r="K15">
+        <v>0.7557755775577558</v>
+      </c>
+      <c r="L15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" t="s">
+        <v>67</v>
+      </c>
+      <c r="N15" t="s">
+        <v>71</v>
+      </c>
+      <c r="O15">
+        <v>425</v>
+      </c>
+      <c r="P15">
+        <v>0.8188235294117647</v>
+      </c>
+      <c r="Q15">
+        <v>0.6826439717571468</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16">
+        <v>976</v>
+      </c>
+      <c r="F16">
+        <v>0.6926229508196722</v>
+      </c>
+      <c r="G16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" t="s">
+        <v>62</v>
+      </c>
+      <c r="J16">
+        <v>743</v>
+      </c>
+      <c r="K16">
+        <v>0.7402422611036339</v>
+      </c>
+      <c r="L16" t="s">
         <v>28</v>
       </c>
-      <c r="D15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15">
-        <v>1159</v>
-      </c>
-      <c r="F15">
-        <v>0.8731665228645384</v>
-      </c>
-      <c r="G15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" t="s">
-        <v>39</v>
-      </c>
-      <c r="J15">
-        <v>911</v>
-      </c>
-      <c r="K15">
-        <v>0.8902305159165752</v>
-      </c>
-      <c r="L15" t="s">
-        <v>18</v>
-      </c>
-      <c r="M15" t="s">
-        <v>40</v>
-      </c>
-      <c r="N15" t="s">
-        <v>44</v>
-      </c>
-      <c r="O15">
-        <v>644</v>
-      </c>
-      <c r="P15">
-        <v>0.8850931677018633</v>
-      </c>
-      <c r="Q15">
-        <v>0.5145413016918816</v>
+      <c r="M16" t="s">
+        <v>68</v>
+      </c>
+      <c r="N16" t="s">
+        <v>61</v>
+      </c>
+      <c r="O16">
+        <v>413</v>
+      </c>
+      <c r="P16">
+        <v>0.8087167070217918</v>
+      </c>
+      <c r="Q16">
+        <v>0.7041483036414198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final iteration of code
</commit_message>
<xml_diff>
--- a/SCALARSelectedandConvertedStatements_PA.xlsx
+++ b/SCALARSelectedandConvertedStatements_PA.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="72">
   <si>
     <t>Attribute</t>
   </si>
@@ -50,31 +50,58 @@
     <t>People living in the Netherlands</t>
   </si>
   <si>
+    <t>R2_implementation_SM1</t>
+  </si>
+  <si>
+    <t>R2_implementation_SM2</t>
+  </si>
+  <si>
     <t>R2_implementation_SM3</t>
   </si>
   <si>
-    <t>R2_implementation_SM6</t>
-  </si>
-  <si>
-    <t>(None,)</t>
+    <t>R2_implementation_NM2</t>
+  </si>
+  <si>
+    <t>R2_implementation_NM3</t>
+  </si>
+  <si>
+    <t>R2_implementation_NM6</t>
+  </si>
+  <si>
+    <t>R1c_perc_cost_SM1</t>
+  </si>
+  <si>
+    <t>R05_worry</t>
+  </si>
+  <si>
+    <t>Q0_age</t>
+  </si>
+  <si>
+    <t>R1c_perc_cost_SM2</t>
+  </si>
+  <si>
+    <t>R1a_self_efficacy_SM3</t>
   </si>
   <si>
     <t>R1c_perc_cost_SM3</t>
   </si>
   <si>
-    <t>R1a_self_efficacy_SM3</t>
-  </si>
-  <si>
-    <t>R1c_perc_cost_SM6</t>
-  </si>
-  <si>
-    <t>R1a_self_efficacy_SM6</t>
-  </si>
-  <si>
-    <t>R01_resilience_6</t>
-  </si>
-  <si>
-    <t>R08_economic_comfort</t>
+    <t>R1c_perc_cost_NM3</t>
+  </si>
+  <si>
+    <t>R1a_self_efficacy_NM6</t>
+  </si>
+  <si>
+    <t>R1a_self_efficacy_SM1</t>
+  </si>
+  <si>
+    <t>R1a_self_efficacy_SM2</t>
+  </si>
+  <si>
+    <t>R1a_self_efficacy_NM3</t>
+  </si>
+  <si>
+    <t>R1c_perc_cost_NM6</t>
   </si>
   <si>
     <t>Aim_description</t>
@@ -98,64 +125,112 @@
     <t>final_entropy</t>
   </si>
   <si>
+    <t>Raising the level of the ground floor above the most likely flood level, Please indicate if you have already implemented any of these structural measures or if you intend to do so in the future</t>
+  </si>
+  <si>
+    <t>Strengthen the housing foundations to withstand water pressures, Please indicate if you have already implemented any of these structural measures or if you intend to do so in the future</t>
+  </si>
+  <si>
     <t>Reconstructing or reinforcing the walls and/or the ground floor with water-resistant materials, Please indicate if you have already implemented any of these structural measures or if you intend to do so in the future</t>
   </si>
   <si>
-    <t>Installing a pump and/or one or more system(s) to drain flood water, Please indicate if you have already implemented any of these structural measures or if you intend to do so in the future</t>
-  </si>
-  <si>
-    <t>not reconstruct or reinforce walls and/or ground floor with water-resistant materials within the next year</t>
-  </si>
-  <si>
-    <t>not install a pump and/or one or more systems to drain flood water within the next year</t>
+    <t>Purchasing sandbags, or other water barriers, Please indicate if you have already implemented any of these nonstructural measures or if you intend to do so in the future</t>
+  </si>
+  <si>
+    <t>Buying a spare power generator to power your home, Please indicate if you have already implemented any of these nonstructural measures or if you intend to do so in the future</t>
+  </si>
+  <si>
+    <t>Installing a refuge zone, or an opening in the roof of your home or apartment, Please indicate if you have already implemented any of these nonstructural measures or if you intend to do so in the future</t>
+  </si>
+  <si>
+    <t>not raise the level of the ground floor above the most likely flood level</t>
+  </si>
+  <si>
+    <t>not strengthen the housing foundations to withstand water pressures</t>
+  </si>
+  <si>
+    <t>not reconstruct or reinforce the walls and/or the ground floor with water-resistant materials</t>
+  </si>
+  <si>
+    <t>not purchase sandbags or other water barriers</t>
+  </si>
+  <si>
+    <t>not buy a spare power generator to power their home</t>
+  </si>
+  <si>
+    <t>not install a refuge zone</t>
+  </si>
+  <si>
+    <t>Raising the level of the ground floor above the most likely flood level, When you think in terms of your income and your other expenses, do you believe that implementing or paying someone to implement this structural measure would be cheap or expensive?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How worried or not are you about the potential impact of flooding on your home?, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age, </t>
+  </si>
+  <si>
+    <t>Strengthen the housing foundations to withstand water pressures, When you think in terms of your income and your other expenses, do you believe that implementing or paying someone to implement this structural measure would be cheap or expensive?</t>
+  </si>
+  <si>
+    <t>Reconstructing or reinforcing the walls and/or the ground floor with water-resistant materials, Do you have the ability to undertake the structural measure either yourself or by paying a professional to do so?</t>
   </si>
   <si>
     <t>Reconstructing or reinforcing the walls and/or the ground floor with water-resistant materials, When you think in terms of your income and your other expenses, do you believe that implementing or paying someone to implement this structural measure would be cheap or expensive?</t>
   </si>
   <si>
-    <t>Reconstructing or reinforcing the walls and/or the ground floor with water-resistant materials, Do you have the ability to undertake the structural measure either yourself or by paying a professional to do so?</t>
-  </si>
-  <si>
-    <t>Installing a pump and/or one or more system(s) to drain flood water, When you think in terms of your income and your other expenses, do you believe that implementing or paying someone to implement this structural measure would be cheap or expensive?</t>
-  </si>
-  <si>
-    <t>Installing a pump and/or one or more system(s) to drain flood water, Do you have the ability to undertake the structural measure either yourself or by paying a professional to do so?</t>
+    <t>Buying a spare power generator to power your home, When you think in terms of your income and your other expenses, do you believe that implementing or paying someone to implement this nonstructural measure would be cheap or expensive?</t>
+  </si>
+  <si>
+    <t>Installing a refuge zone, or an opening in the roof of your home or apartment, Do you have the ability to undertake the nonstructural measure either yourself or by paying a professional to do so?</t>
+  </si>
+  <si>
+    <t>if they believe that implementing or paying someone to implement this structural measure would be expensive</t>
+  </si>
+  <si>
+    <t>if they are not worried about the potential impact of flooding on their home</t>
+  </si>
+  <si>
+    <t>if they are younger than 45</t>
+  </si>
+  <si>
+    <t>if they are older than 45</t>
+  </si>
+  <si>
+    <t>if they are not able to undertake the structural measure either themselves or by paying a professional to do so</t>
+  </si>
+  <si>
+    <t>if they believe that implementing or paying someone to implement this nonstructural measure would be expensive</t>
+  </si>
+  <si>
+    <t>if they are not able to install a refuge zone or an opening in the roof of their home or apartment</t>
+  </si>
+  <si>
+    <t>Raising the level of the ground floor above the most likely flood level</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Strengthen the housing foundations to withstand water pressures</t>
+  </si>
+  <si>
+    <t>Reconstructing or reinforcing the walls and/or the ground floor with water-resistant materials</t>
+  </si>
+  <si>
+    <t>Buying a spare power generator to power your home</t>
+  </si>
+  <si>
+    <t>Installing a refuge zone, or an opening in the roof of your home or apartment</t>
   </si>
   <si>
     <t>None</t>
   </si>
   <si>
-    <t>if they believe that implementing or paying someone to implement this structural measure would be cheap</t>
-  </si>
-  <si>
-    <t>if they believe that implementing or paying someone to implement this structural measure would be expensive</t>
-  </si>
-  <si>
-    <t>if they are not able to undertake the structural measure either themselves or by paying a professional to do so</t>
-  </si>
-  <si>
-    <t>if they do not have the ability to undertake the structural measure either themselves or by paying a professional to do so</t>
-  </si>
-  <si>
-    <t>My household can rely on the support from my government when I need help (e.g. receiving funding or support in the event of a natural disaster)</t>
-  </si>
-  <si>
-    <t>Reconstructing or reinforcing the walls and/or the ground floor with water-resistant materials</t>
-  </si>
-  <si>
-    <t>When considering your salary along with your expenses, how would you describe your level of 'economic comfort'?</t>
-  </si>
-  <si>
-    <t>Installing a pump and/or one or more system(s) to drain flood water</t>
-  </si>
-  <si>
-    <t>if they feel they can rely on government support</t>
-  </si>
-  <si>
-    <t>if they feel they cannot rely on government support</t>
-  </si>
-  <si>
-    <t>if they feel they are not living comfortably</t>
+    <t>if they are not able to</t>
+  </si>
+  <si>
+    <t>if they are not able to buy a spare power generator to power their home</t>
   </si>
 </sst>
 </file>
@@ -513,7 +588,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -559,28 +634,25 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D2">
-        <v>0.8930112165660051</v>
+        <v>0.7684426229508197</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F2">
-        <v>1159</v>
+        <v>632</v>
       </c>
       <c r="G2">
-        <v>0.8930112165660051</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
+        <v>0.8908227848101266</v>
       </c>
       <c r="I2">
-        <v>1159</v>
+        <v>632</v>
       </c>
       <c r="J2">
-        <v>0.8930112165660051</v>
+        <v>0.8908227848101266</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -591,28 +663,28 @@
         <v>11</v>
       </c>
       <c r="C3">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D3">
-        <v>0.8930112165660051</v>
+        <v>0.7684426229508197</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F3">
-        <v>416</v>
+        <v>632</v>
       </c>
       <c r="G3">
-        <v>0.7788461538461539</v>
+        <v>0.8908227848101266</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I3">
-        <v>311</v>
+        <v>572</v>
       </c>
       <c r="J3">
-        <v>0.7877813504823151</v>
+        <v>0.9265734265734266</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -623,25 +695,25 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D4">
-        <v>0.8930112165660051</v>
+        <v>0.7684426229508197</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F4">
-        <v>743</v>
+        <v>863</v>
       </c>
       <c r="G4">
-        <v>0.9569313593539704</v>
+        <v>0.813441483198146</v>
       </c>
       <c r="I4">
-        <v>743</v>
+        <v>863</v>
       </c>
       <c r="J4">
-        <v>0.9569313593539704</v>
+        <v>0.813441483198146</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -652,28 +724,28 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D5">
-        <v>0.8930112165660051</v>
+        <v>0.7684426229508197</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F5">
-        <v>743</v>
+        <v>863</v>
       </c>
       <c r="G5">
-        <v>0.9569313593539704</v>
+        <v>0.813441483198146</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="I5">
-        <v>635</v>
+        <v>381</v>
       </c>
       <c r="J5">
-        <v>0.9732283464566929</v>
+        <v>0.916010498687664</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -681,28 +753,31 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D6">
-        <v>0.8930112165660051</v>
+        <v>0.7725409836065574</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F6">
-        <v>974</v>
+        <v>564</v>
       </c>
       <c r="G6">
-        <v>0.9065708418891171</v>
+        <v>0.6790780141843972</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
       </c>
       <c r="I6">
-        <v>974</v>
+        <v>357</v>
       </c>
       <c r="J6">
-        <v>0.9065708418891171</v>
+        <v>0.7871148459383753</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -710,31 +785,28 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D7">
-        <v>0.8930112165660051</v>
+        <v>0.7725409836065574</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F7">
-        <v>974</v>
+        <v>412</v>
       </c>
       <c r="G7">
-        <v>0.9065708418891171</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
+        <v>0.9004854368932039</v>
       </c>
       <c r="I7">
-        <v>680</v>
+        <v>412</v>
       </c>
       <c r="J7">
-        <v>0.9058823529411765</v>
+        <v>0.9004854368932039</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -742,31 +814,31 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D8">
-        <v>0.8930112165660051</v>
+        <v>0.7725409836065574</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F8">
-        <v>974</v>
+        <v>412</v>
       </c>
       <c r="G8">
-        <v>0.9065708418891171</v>
+        <v>0.9004854368932039</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I8">
-        <v>294</v>
+        <v>387</v>
       </c>
       <c r="J8">
-        <v>0.9081632653061225</v>
+        <v>0.9198966408268734</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -777,28 +849,25 @@
         <v>12</v>
       </c>
       <c r="C9">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D9">
-        <v>0.8731665228645384</v>
+        <v>0.7725409836065574</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F9">
-        <v>1159</v>
+        <v>654</v>
       </c>
       <c r="G9">
-        <v>0.8731665228645384</v>
-      </c>
-      <c r="H9" t="s">
-        <v>13</v>
+        <v>0.8532110091743119</v>
       </c>
       <c r="I9">
-        <v>1159</v>
+        <v>654</v>
       </c>
       <c r="J9">
-        <v>0.8731665228645384</v>
+        <v>0.8532110091743119</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -809,25 +878,28 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D10">
-        <v>0.8731665228645384</v>
+        <v>0.7725409836065574</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F10">
-        <v>572</v>
+        <v>654</v>
       </c>
       <c r="G10">
-        <v>0.8234265734265734</v>
+        <v>0.8532110091743119</v>
+      </c>
+      <c r="H10" t="s">
+        <v>26</v>
       </c>
       <c r="I10">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J10">
-        <v>0.8234265734265734</v>
+        <v>0.8896672504378283</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -835,31 +907,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D11">
-        <v>0.8731665228645384</v>
+        <v>0.757172131147541</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F11">
-        <v>572</v>
+        <v>822</v>
       </c>
       <c r="G11">
-        <v>0.8234265734265734</v>
-      </c>
-      <c r="H11" t="s">
-        <v>19</v>
+        <v>0.818734793187348</v>
       </c>
       <c r="I11">
-        <v>291</v>
+        <v>822</v>
       </c>
       <c r="J11">
-        <v>0.8075601374570447</v>
+        <v>0.818734793187348</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -867,28 +936,31 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D12">
-        <v>0.8731665228645384</v>
+        <v>0.757172131147541</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F12">
-        <v>587</v>
+        <v>822</v>
       </c>
       <c r="G12">
-        <v>0.9216354344122658</v>
+        <v>0.818734793187348</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
       </c>
       <c r="I12">
-        <v>587</v>
+        <v>537</v>
       </c>
       <c r="J12">
-        <v>0.9216354344122658</v>
+        <v>0.9199255121042831</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -896,31 +968,28 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D13">
-        <v>0.8731665228645384</v>
+        <v>0.757172131147541</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F13">
-        <v>587</v>
+        <v>633</v>
       </c>
       <c r="G13">
-        <v>0.9216354344122658</v>
-      </c>
-      <c r="H13" t="s">
-        <v>17</v>
+        <v>0.8499210110584519</v>
       </c>
       <c r="I13">
-        <v>468</v>
+        <v>633</v>
       </c>
       <c r="J13">
-        <v>0.9487179487179487</v>
+        <v>0.8499210110584519</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -928,28 +997,31 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C14">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D14">
-        <v>0.8731665228645384</v>
+        <v>0.6987704918032787</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F14">
-        <v>911</v>
+        <v>863</v>
       </c>
       <c r="G14">
-        <v>0.8902305159165752</v>
+        <v>0.7323290845886443</v>
+      </c>
+      <c r="H14" t="s">
+        <v>19</v>
       </c>
       <c r="I14">
-        <v>911</v>
+        <v>381</v>
       </c>
       <c r="J14">
-        <v>0.8902305159165752</v>
+        <v>0.8083989501312336</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -957,31 +1029,63 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C15">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="D15">
-        <v>0.8731665228645384</v>
+        <v>0.6875</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F15">
-        <v>911</v>
+        <v>606</v>
       </c>
       <c r="G15">
-        <v>0.8902305159165752</v>
+        <v>0.7557755775577558</v>
       </c>
       <c r="H15" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="I15">
-        <v>644</v>
+        <v>425</v>
       </c>
       <c r="J15">
-        <v>0.8850931677018633</v>
+        <v>0.8188235294117647</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>976</v>
+      </c>
+      <c r="D16">
+        <v>0.6926229508196722</v>
+      </c>
+      <c r="E16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16">
+        <v>743</v>
+      </c>
+      <c r="G16">
+        <v>0.7402422611036339</v>
+      </c>
+      <c r="H16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16">
+        <v>413</v>
+      </c>
+      <c r="J16">
+        <v>0.8087167070217918</v>
       </c>
     </row>
   </sheetData>
@@ -991,7 +1095,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1005,10 +1109,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1020,10 +1124,10 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>5</v>
@@ -1035,10 +1139,10 @@
         <v>7</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>8</v>
@@ -1047,7 +1151,7 @@
         <v>9</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1058,43 +1162,43 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="E2">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F2">
-        <v>0.8930112165660051</v>
+        <v>0.7684426229508197</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>48</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="J2">
-        <v>1159</v>
+        <v>632</v>
       </c>
       <c r="K2">
-        <v>0.8930112165660051</v>
-      </c>
-      <c r="L2" t="s">
-        <v>13</v>
+        <v>0.8908227848101266</v>
       </c>
       <c r="N2" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="O2">
-        <v>1159</v>
+        <v>632</v>
       </c>
       <c r="P2">
-        <v>0.8930112165660051</v>
+        <v>0.8908227848101266</v>
       </c>
       <c r="Q2">
-        <v>0.4907658676516883</v>
+        <v>0.4974291918181426</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1105,49 +1209,49 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="E3">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F3">
-        <v>0.8930112165660051</v>
+        <v>0.7684426229508197</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="J3">
-        <v>416</v>
+        <v>632</v>
       </c>
       <c r="K3">
-        <v>0.7788461538461539</v>
+        <v>0.8908227848101266</v>
       </c>
       <c r="L3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="M3" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="N3" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="O3">
-        <v>311</v>
+        <v>572</v>
       </c>
       <c r="P3">
-        <v>0.7877813504823151</v>
+        <v>0.9265734265734266</v>
       </c>
       <c r="Q3">
-        <v>0.7457022590910922</v>
+        <v>0.3785827651603728</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -1158,43 +1262,43 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="E4">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F4">
-        <v>0.8930112165660051</v>
+        <v>0.7684426229508197</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="I4" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="J4">
-        <v>743</v>
+        <v>863</v>
       </c>
       <c r="K4">
-        <v>0.9569313593539704</v>
+        <v>0.813441483198146</v>
       </c>
       <c r="N4" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="O4">
-        <v>743</v>
+        <v>863</v>
       </c>
       <c r="P4">
-        <v>0.9569313593539704</v>
+        <v>0.813441483198146</v>
       </c>
       <c r="Q4">
-        <v>0.256189076205616</v>
+        <v>0.6942163713918693</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -1205,49 +1309,49 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="E5">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F5">
-        <v>0.8930112165660051</v>
+        <v>0.7684426229508197</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="J5">
-        <v>743</v>
+        <v>863</v>
       </c>
       <c r="K5">
-        <v>0.9569313593539704</v>
+        <v>0.813441483198146</v>
       </c>
       <c r="L5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="M5" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="N5" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="O5">
-        <v>635</v>
+        <v>381</v>
       </c>
       <c r="P5">
-        <v>0.9732283464566929</v>
+        <v>0.916010498687664</v>
       </c>
       <c r="Q5">
-        <v>0.1779340107206948</v>
+        <v>0.4160827624351366</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1255,46 +1359,52 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E6">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F6">
-        <v>0.8930112165660051</v>
+        <v>0.7725409836065574</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="J6">
-        <v>974</v>
+        <v>564</v>
       </c>
       <c r="K6">
-        <v>0.9065708418891171</v>
+        <v>0.6790780141843972</v>
+      </c>
+      <c r="L6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" t="s">
+        <v>65</v>
       </c>
       <c r="N6" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="O6">
-        <v>974</v>
+        <v>357</v>
       </c>
       <c r="P6">
-        <v>0.9065708418891171</v>
+        <v>0.7871148459383753</v>
       </c>
       <c r="Q6">
-        <v>0.4478134923988957</v>
+        <v>0.7469615329260388</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1302,52 +1412,46 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E7">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F7">
-        <v>0.8930112165660051</v>
+        <v>0.7725409836065574</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="J7">
-        <v>974</v>
+        <v>412</v>
       </c>
       <c r="K7">
-        <v>0.9065708418891171</v>
-      </c>
-      <c r="L7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7" t="s">
-        <v>40</v>
+        <v>0.9004854368932039</v>
       </c>
       <c r="N7" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="O7">
-        <v>680</v>
+        <v>412</v>
       </c>
       <c r="P7">
-        <v>0.9058823529411765</v>
+        <v>0.9004854368932039</v>
       </c>
       <c r="Q7">
-        <v>0.4500666580964382</v>
+        <v>0.4674549036015206</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1355,52 +1459,52 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="E8">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F8">
-        <v>0.8930112165660051</v>
+        <v>0.7725409836065574</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="I8" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="J8">
-        <v>974</v>
+        <v>412</v>
       </c>
       <c r="K8">
-        <v>0.9065708418891171</v>
+        <v>0.9004854368932039</v>
       </c>
       <c r="L8" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="M8" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="N8" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="O8">
-        <v>294</v>
+        <v>387</v>
       </c>
       <c r="P8">
-        <v>0.9081632653061225</v>
+        <v>0.9198966408268734</v>
       </c>
       <c r="Q8">
-        <v>0.4425710648397979</v>
+        <v>0.4025432779892922</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1411,43 +1515,43 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E9">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F9">
-        <v>0.8731665228645384</v>
+        <v>0.7725409836065574</v>
       </c>
       <c r="G9" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>51</v>
       </c>
       <c r="I9" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="J9">
-        <v>1159</v>
+        <v>654</v>
       </c>
       <c r="K9">
-        <v>0.8731665228645384</v>
-      </c>
-      <c r="L9" t="s">
-        <v>13</v>
+        <v>0.8532110091743119</v>
       </c>
       <c r="N9" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="O9">
-        <v>1159</v>
+        <v>654</v>
       </c>
       <c r="P9">
-        <v>0.8731665228645384</v>
+        <v>0.8532110091743119</v>
       </c>
       <c r="Q9">
-        <v>0.5486895858799942</v>
+        <v>0.6017460730975969</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1458,43 +1562,49 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E10">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F10">
-        <v>0.8731665228645384</v>
+        <v>0.7725409836065574</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H10" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="I10" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="J10">
-        <v>572</v>
+        <v>654</v>
       </c>
       <c r="K10">
-        <v>0.8234265734265734</v>
+        <v>0.8532110091743119</v>
+      </c>
+      <c r="L10" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" t="s">
+        <v>65</v>
       </c>
       <c r="N10" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="O10">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="P10">
-        <v>0.8234265734265734</v>
+        <v>0.8896672504378283</v>
       </c>
       <c r="Q10">
-        <v>0.6725233117337178</v>
+        <v>0.5009188161671247</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1502,52 +1612,46 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E11">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F11">
-        <v>0.8731665228645384</v>
+        <v>0.757172131147541</v>
       </c>
       <c r="G11" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H11" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="I11" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="J11">
-        <v>572</v>
+        <v>822</v>
       </c>
       <c r="K11">
-        <v>0.8234265734265734</v>
-      </c>
-      <c r="L11" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" t="s">
-        <v>42</v>
+        <v>0.818734793187348</v>
       </c>
       <c r="N11" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="O11">
-        <v>291</v>
+        <v>822</v>
       </c>
       <c r="P11">
-        <v>0.8075601374570447</v>
+        <v>0.818734793187348</v>
       </c>
       <c r="Q11">
-        <v>0.7065476519185905</v>
+        <v>0.6828370374266884</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1555,46 +1659,52 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E12">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F12">
-        <v>0.8731665228645384</v>
+        <v>0.757172131147541</v>
       </c>
       <c r="G12" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H12" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="I12" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="J12">
-        <v>587</v>
+        <v>822</v>
       </c>
       <c r="K12">
-        <v>0.9216354344122658</v>
+        <v>0.818734793187348</v>
+      </c>
+      <c r="L12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" t="s">
+        <v>66</v>
       </c>
       <c r="N12" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="O12">
-        <v>587</v>
+        <v>537</v>
       </c>
       <c r="P12">
-        <v>0.9216354344122658</v>
+        <v>0.9199255121042831</v>
       </c>
       <c r="Q12">
-        <v>0.3963902569449249</v>
+        <v>0.4024415985533437</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1602,52 +1712,46 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E13">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F13">
-        <v>0.8731665228645384</v>
+        <v>0.757172131147541</v>
       </c>
       <c r="G13" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H13" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="I13" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="J13">
-        <v>587</v>
+        <v>633</v>
       </c>
       <c r="K13">
-        <v>0.9216354344122658</v>
-      </c>
-      <c r="L13" t="s">
-        <v>17</v>
-      </c>
-      <c r="M13" t="s">
-        <v>43</v>
+        <v>0.8499210110584519</v>
       </c>
       <c r="N13" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="O13">
-        <v>468</v>
+        <v>633</v>
       </c>
       <c r="P13">
-        <v>0.9487179487179487</v>
+        <v>0.8499210110584519</v>
       </c>
       <c r="Q13">
-        <v>0.2918182565988858</v>
+        <v>0.6100379392752546</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1655,46 +1759,52 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E14">
-        <v>1159</v>
+        <v>976</v>
       </c>
       <c r="F14">
-        <v>0.8731665228645384</v>
+        <v>0.6987704918032787</v>
       </c>
       <c r="G14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H14" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="I14" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="J14">
-        <v>911</v>
+        <v>863</v>
       </c>
       <c r="K14">
-        <v>0.8902305159165752</v>
+        <v>0.7323290845886443</v>
+      </c>
+      <c r="L14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" t="s">
+        <v>64</v>
       </c>
       <c r="N14" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="O14">
-        <v>911</v>
+        <v>381</v>
       </c>
       <c r="P14">
-        <v>0.8902305159165752</v>
+        <v>0.8083989501312336</v>
       </c>
       <c r="Q14">
-        <v>0.4992202608188665</v>
+        <v>0.7048087430516662</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1702,52 +1812,105 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15">
+        <v>976</v>
+      </c>
+      <c r="F15">
+        <v>0.6875</v>
+      </c>
+      <c r="G15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15">
+        <v>606</v>
+      </c>
+      <c r="K15">
+        <v>0.7557755775577558</v>
+      </c>
+      <c r="L15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" t="s">
+        <v>67</v>
+      </c>
+      <c r="N15" t="s">
+        <v>71</v>
+      </c>
+      <c r="O15">
+        <v>425</v>
+      </c>
+      <c r="P15">
+        <v>0.8188235294117647</v>
+      </c>
+      <c r="Q15">
+        <v>0.6826439717571468</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16">
+        <v>976</v>
+      </c>
+      <c r="F16">
+        <v>0.6926229508196722</v>
+      </c>
+      <c r="G16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" t="s">
+        <v>62</v>
+      </c>
+      <c r="J16">
+        <v>743</v>
+      </c>
+      <c r="K16">
+        <v>0.7402422611036339</v>
+      </c>
+      <c r="L16" t="s">
         <v>28</v>
       </c>
-      <c r="D15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15">
-        <v>1159</v>
-      </c>
-      <c r="F15">
-        <v>0.8731665228645384</v>
-      </c>
-      <c r="G15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" t="s">
-        <v>39</v>
-      </c>
-      <c r="J15">
-        <v>911</v>
-      </c>
-      <c r="K15">
-        <v>0.8902305159165752</v>
-      </c>
-      <c r="L15" t="s">
-        <v>18</v>
-      </c>
-      <c r="M15" t="s">
-        <v>40</v>
-      </c>
-      <c r="N15" t="s">
-        <v>44</v>
-      </c>
-      <c r="O15">
-        <v>644</v>
-      </c>
-      <c r="P15">
-        <v>0.8850931677018633</v>
-      </c>
-      <c r="Q15">
-        <v>0.5145413016918816</v>
+      <c r="M16" t="s">
+        <v>68</v>
+      </c>
+      <c r="N16" t="s">
+        <v>61</v>
+      </c>
+      <c r="O16">
+        <v>413</v>
+      </c>
+      <c r="P16">
+        <v>0.8087167070217918</v>
+      </c>
+      <c r="Q16">
+        <v>0.7041483036414198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>